<commit_message>
Succeful test when given all branch information
</commit_message>
<xml_diff>
--- a/src/test_results.xlsx
+++ b/src/test_results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-32000" yWindow="-440" windowWidth="32000" windowHeight="23540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,9 +44,6 @@
     <t>t</t>
   </si>
   <si>
-    <t>OBJ = 99.76688640508485</t>
-  </si>
-  <si>
     <t>lb</t>
   </si>
   <si>
@@ -54,6 +51,9 @@
   </si>
   <si>
     <t>iter</t>
+  </si>
+  <si>
+    <t>OBJ = 100.54302354521576</t>
   </si>
 </sst>
 </file>
@@ -377,8 +377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -391,16 +391,16 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="L1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" t="s">
         <v>6</v>
-      </c>
-      <c r="N1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
@@ -425,23 +425,23 @@
         <v>0</v>
       </c>
       <c r="B3">
-        <v>93.143553578124298</v>
+        <v>92.741201823774205</v>
       </c>
       <c r="F3" s="1">
-        <v>100.905290152663</v>
+        <v>103.296670310378</v>
       </c>
       <c r="G3" s="1">
-        <v>99.503955493103206</v>
+        <v>103.32544238673999</v>
       </c>
       <c r="H3" s="1">
-        <v>97.775972199307603</v>
+        <v>98.372469602169303</v>
       </c>
       <c r="I3" s="1">
-        <v>103.826031253913</v>
+        <v>100.64498820221399</v>
       </c>
       <c r="J3">
         <f>0.1*B3+0.225*(SUM(F3:I3))</f>
-        <v>99.766886405084463</v>
+        <v>100.54302354521521</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
@@ -529,19 +529,19 @@
         <v>5</v>
       </c>
       <c r="B8">
-        <v>19.999999999999901</v>
+        <v>28.203592386740699</v>
       </c>
       <c r="F8" s="1">
-        <v>20.000000000000199</v>
+        <v>28.203592386740699</v>
       </c>
       <c r="G8" s="1">
-        <v>20.000000000000199</v>
+        <v>28.203592386740699</v>
       </c>
       <c r="H8" s="1">
-        <v>20.000000000000199</v>
+        <v>28.203592386740699</v>
       </c>
       <c r="I8" s="1">
-        <v>20.000000000000199</v>
+        <v>28.203592386740699</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
@@ -549,19 +549,19 @@
         <v>6</v>
       </c>
       <c r="B9">
-        <v>15</v>
+        <v>19.203592386740699</v>
       </c>
       <c r="F9" s="1">
-        <v>15</v>
+        <v>19.203592386740699</v>
       </c>
       <c r="G9" s="1">
-        <v>15</v>
+        <v>19.203592386740699</v>
       </c>
       <c r="H9" s="1">
-        <v>15</v>
+        <v>19.203592386740699</v>
       </c>
       <c r="I9" s="1">
-        <v>15</v>
+        <v>19.203592386740699</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
@@ -569,19 +569,19 @@
         <v>7</v>
       </c>
       <c r="B10">
-        <v>15</v>
+        <v>19.203592386740699</v>
       </c>
       <c r="F10" s="1">
-        <v>14.999999999999901</v>
+        <v>19.203592386740699</v>
       </c>
       <c r="G10" s="1">
-        <v>15</v>
+        <v>19.203592386740699</v>
       </c>
       <c r="H10" s="1">
-        <v>15</v>
+        <v>19.203592386740699</v>
       </c>
       <c r="I10" s="1">
-        <v>15</v>
+        <v>19.203592386740699</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
@@ -589,19 +589,19 @@
         <v>8</v>
       </c>
       <c r="B11">
-        <v>34.999999999999901</v>
+        <v>43.203592386740702</v>
       </c>
       <c r="F11" s="1">
-        <v>35.000000000000199</v>
+        <v>43.203592386740702</v>
       </c>
       <c r="G11" s="1">
-        <v>35.000000000000199</v>
+        <v>43.203592386740702</v>
       </c>
       <c r="H11" s="1">
-        <v>35.000000000000199</v>
+        <v>43.203592386740702</v>
       </c>
       <c r="I11" s="1">
-        <v>35.000000000000199</v>
+        <v>43.203592386740702</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
@@ -609,119 +609,119 @@
         <v>9</v>
       </c>
       <c r="B12">
-        <v>35</v>
+        <v>43.203592386740702</v>
       </c>
       <c r="F12" s="1">
-        <v>35</v>
+        <v>46.210770310378599</v>
       </c>
       <c r="G12" s="1">
-        <v>35</v>
+        <v>43.203592386740702</v>
       </c>
       <c r="H12" s="1">
-        <v>35.446972199307602</v>
+        <v>43.203592386740702</v>
       </c>
       <c r="I12" s="1">
-        <v>46.908472199307603</v>
+        <v>43.203592386740702</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
+      <c r="A13">
         <v>10</v>
       </c>
       <c r="B13">
-        <v>45</v>
+        <v>49.203592386740702</v>
       </c>
       <c r="F13" s="1">
-        <v>45</v>
+        <v>49.203592386740702</v>
       </c>
       <c r="G13" s="1">
-        <v>45</v>
+        <v>49.203592386740702</v>
       </c>
       <c r="H13" s="1">
-        <v>45</v>
+        <v>49.203592386740702</v>
       </c>
       <c r="I13" s="1">
-        <v>52.079772199307598</v>
+        <v>52.050042386740699</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
+      <c r="A14">
         <v>11</v>
       </c>
       <c r="B14">
-        <v>35</v>
+        <v>43.203592386740702</v>
       </c>
       <c r="F14" s="1">
-        <v>35</v>
+        <v>43.203592386740702</v>
       </c>
       <c r="G14" s="1">
-        <v>35</v>
+        <v>43.203592386740702</v>
       </c>
       <c r="H14" s="1">
-        <v>35</v>
+        <v>43.203592386740702</v>
       </c>
       <c r="I14" s="1">
-        <v>35</v>
+        <v>43.203592386740702</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
+      <c r="A15">
         <v>12</v>
       </c>
       <c r="B15">
-        <v>63.143553578124298</v>
+        <v>65.703592386740794</v>
       </c>
       <c r="F15" s="1">
-        <v>63.143553578124298</v>
+        <v>76.463792386740707</v>
       </c>
       <c r="G15" s="1">
-        <v>63.143553578124298</v>
+        <v>82.836992386740803</v>
       </c>
       <c r="H15" s="1">
-        <v>67.1066</v>
+        <v>71.054819602169303</v>
       </c>
       <c r="I15" s="1">
-        <v>57.368000000000002</v>
+        <v>65.571592386740804</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
+      <c r="A16">
         <v>13</v>
       </c>
       <c r="B16">
-        <v>75</v>
+        <v>77.241201823774205</v>
       </c>
       <c r="F16" s="1">
-        <v>74.953172199307602</v>
+        <v>75.769870310378593</v>
       </c>
       <c r="G16" s="1">
-        <v>73.985455493103203</v>
+        <v>77.806942386740801</v>
       </c>
       <c r="H16" s="1">
-        <v>74.953172199307602</v>
+        <v>82.709792386740702</v>
       </c>
       <c r="I16" s="1">
-        <v>74.953172199307602</v>
+        <v>74.923442386740703</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
+      <c r="A17">
         <v>14</v>
       </c>
       <c r="B17">
-        <v>88.143553578124298</v>
+        <v>87.741201823774205</v>
       </c>
       <c r="F17" s="1">
-        <v>93.1806901526638</v>
+        <v>95.572070310378606</v>
       </c>
       <c r="G17" s="1">
-        <v>95.613555493103206</v>
+        <v>99.435042386740804</v>
       </c>
       <c r="H17" s="1">
-        <v>92.097472199307603</v>
+        <v>92.693969602169304</v>
       </c>
       <c r="I17" s="1">
-        <v>96.979131253913806</v>
+        <v>93.798088202214799</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -784,21 +784,21 @@
       <c r="B22">
         <v>1</v>
       </c>
-      <c r="C22">
-        <v>0.79999999999998095</v>
+      <c r="C22" s="1">
+        <v>0.14371260906073599</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1">
-        <v>0.79999999999998095</v>
+        <v>0.14371260906073599</v>
       </c>
       <c r="G22" s="1">
-        <v>0.79999999999998095</v>
+        <v>0.14371260906073599</v>
       </c>
       <c r="H22" s="1">
-        <v>0.79999999999998095</v>
+        <v>0.14371260906073599</v>
       </c>
       <c r="I22" s="1">
-        <v>0.79999999999998095</v>
+        <v>0.14371260906073599</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
@@ -808,21 +808,21 @@
       <c r="B23">
         <v>1</v>
       </c>
-      <c r="C23">
-        <v>1</v>
+      <c r="C23" s="1">
+        <v>0.57964076132592002</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1">
-        <v>1</v>
+        <v>0.57964076132592002</v>
       </c>
       <c r="G23" s="1">
-        <v>1</v>
+        <v>0.57964076132592002</v>
       </c>
       <c r="H23" s="1">
-        <v>1</v>
+        <v>0.57964076132592002</v>
       </c>
       <c r="I23" s="1">
-        <v>1</v>
+        <v>0.57964076132592002</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
@@ -857,20 +857,20 @@
         <v>1</v>
       </c>
       <c r="C25">
-        <v>0.33333333333333298</v>
+        <v>0</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1">
-        <v>0.33333333333333298</v>
+        <v>0</v>
       </c>
       <c r="G25" s="1">
-        <v>0.33333333333333298</v>
+        <v>0</v>
       </c>
       <c r="H25" s="1">
-        <v>0.33333333333333298</v>
+        <v>0</v>
       </c>
       <c r="I25" s="1">
-        <v>0.33333333333333298</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
@@ -904,21 +904,21 @@
       <c r="B27">
         <v>1</v>
       </c>
-      <c r="C27">
-        <v>0.36925827757928897</v>
+      <c r="C27" s="1">
+        <v>0.61070981889659204</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1">
-        <v>0.36925827757928897</v>
+        <v>0.86969349735220802</v>
       </c>
       <c r="G27" s="1">
-        <v>0.34384229649897802</v>
+        <v>0.53000038233282498</v>
       </c>
       <c r="H27" s="1">
-        <v>0.36925827757928897</v>
+        <v>0.68385493360340599</v>
       </c>
       <c r="I27" s="1">
-        <v>0.36925827757928897</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
@@ -928,8 +928,8 @@
       <c r="B28">
         <v>1</v>
       </c>
-      <c r="C28">
-        <v>0</v>
+      <c r="C28" s="1">
+        <v>0.29811952814832499</v>
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1">
@@ -952,18 +952,18 @@
       <c r="B29">
         <v>1</v>
       </c>
-      <c r="C29">
-        <v>0</v>
+      <c r="C29" s="1">
+        <v>0.130826037531101</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1">
-        <v>0.31223585629843298</v>
+        <v>0.50307636824646595</v>
       </c>
       <c r="G29" s="1">
-        <v>0.72990298630879302</v>
+        <v>0.74664624728051798</v>
       </c>
       <c r="H29" s="1">
-        <v>0.65229997213514102</v>
+        <v>0.49243658156883602</v>
       </c>
       <c r="I29" s="1">
         <v>0</v>
@@ -977,17 +977,17 @@
         <v>1</v>
       </c>
       <c r="C30">
-        <v>0.74917539652780796</v>
+        <v>1</v>
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1">
-        <v>0.74917539652780796</v>
+        <v>1</v>
       </c>
       <c r="G30" s="1">
-        <v>0.74917539652780796</v>
+        <v>1</v>
       </c>
       <c r="H30" s="1">
-        <v>0</v>
+        <v>0.26507775875187101</v>
       </c>
       <c r="I30" s="1">
         <v>1</v>
@@ -1000,21 +1000,21 @@
       <c r="B31">
         <v>1</v>
       </c>
-      <c r="C31">
-        <v>0</v>
+      <c r="C31" s="1">
+        <v>0.236991245037321</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1">
-        <v>0.27695601490658001</v>
+        <v>0.90387676401466799</v>
       </c>
       <c r="G31" s="1">
-        <v>4.3745987331107301E-2</v>
+        <v>1</v>
       </c>
       <c r="H31" s="1">
-        <v>0.84510841695225403</v>
+        <v>1</v>
       </c>
       <c r="I31" s="1">
-        <v>7.3173007976874593E-2</v>
+        <v>0.62696236371412795</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
@@ -1025,20 +1025,20 @@
         <v>1</v>
       </c>
       <c r="C32">
-        <v>0.74823299255958897</v>
+        <v>1</v>
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1">
-        <v>0.15904112135457399</v>
+        <v>0</v>
       </c>
       <c r="G32" s="1">
         <v>0</v>
       </c>
       <c r="H32" s="1">
-        <v>0</v>
+        <v>0.83527735568922801</v>
       </c>
       <c r="I32" s="1">
-        <v>0.42423538111052</v>
+        <v>0.64968426589921402</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
@@ -1068,23 +1068,23 @@
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C34">
         <f>SUM(C20:C33)</f>
-        <v>4</v>
+        <v>3.9999999999999947</v>
       </c>
       <c r="F34">
         <f>SUM(F20:F33)</f>
-        <v>3.9999999999999982</v>
+        <v>3.9999999999999978</v>
       </c>
       <c r="G34">
         <f t="shared" ref="G34:I34" si="0">SUM(G20:G33)</f>
-        <v>4</v>
+        <v>3.9999999999999991</v>
       </c>
       <c r="H34">
         <f t="shared" si="0"/>
-        <v>3.9999999999999982</v>
+        <v>3.9999999999999969</v>
       </c>
       <c r="I34">
         <f t="shared" si="0"/>
-        <v>3.9999999999999973</v>
+        <v>3.9999999999999978</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added the deterministic/expected solving processes
</commit_message>
<xml_diff>
--- a/src/test_results.xlsx
+++ b/src/test_results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16200" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -377,8 +377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -417,7 +417,7 @@
         <v>89.687294844121197</v>
       </c>
       <c r="N2" s="1">
-        <v>101.030635995965</v>
+        <v>101.354109856211</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>